<commit_message>
Data_analysis. Calculo de acciones en USD
</commit_message>
<xml_diff>
--- a/data/quotes/alua.xlsx
+++ b/data/quotes/alua.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H587"/>
+  <dimension ref="A1:H592"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3014,13 +3014,13 @@
         <v>82</v>
       </c>
       <c r="F92" t="n">
-        <v>20163126.5</v>
+        <v>20204953.3</v>
       </c>
       <c r="G92" t="n">
-        <v>500</v>
+        <v>7</v>
       </c>
       <c r="H92" t="n">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="93">
@@ -3042,13 +3042,13 @@
         <v>82.2</v>
       </c>
       <c r="F93" t="n">
-        <v>57805127.3</v>
+        <v>49555690.7</v>
       </c>
       <c r="G93" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H93" t="n">
-        <v>972</v>
+        <v>833</v>
       </c>
     </row>
     <row r="94">
@@ -16834,25 +16834,25 @@
         </is>
       </c>
       <c r="B586" t="n">
-        <v>1002.5</v>
+        <v>1030</v>
       </c>
       <c r="C586" t="n">
         <v>990</v>
       </c>
       <c r="D586" t="n">
-        <v>1019.5</v>
+        <v>1034</v>
       </c>
       <c r="E586" t="n">
-        <v>990</v>
+        <v>953</v>
       </c>
       <c r="F586" t="n">
-        <v>194485919</v>
+        <v>962965672</v>
       </c>
       <c r="G586" t="n">
-        <v>1</v>
+        <v>953186</v>
       </c>
       <c r="H586" t="n">
-        <v>1228</v>
+        <v>3317</v>
       </c>
     </row>
     <row r="587">
@@ -16881,6 +16881,146 @@
       </c>
       <c r="H587" t="n">
         <v>2462</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="B588" t="n">
+        <v>1001.5</v>
+      </c>
+      <c r="C588" t="n">
+        <v>1034</v>
+      </c>
+      <c r="D588" t="n">
+        <v>1035</v>
+      </c>
+      <c r="E588" t="n">
+        <v>995.5</v>
+      </c>
+      <c r="F588" t="n">
+        <v>586738307.5</v>
+      </c>
+      <c r="G588" t="n">
+        <v>583077</v>
+      </c>
+      <c r="H588" t="n">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="B589" t="n">
+        <v>1010</v>
+      </c>
+      <c r="C589" t="n">
+        <v>1002</v>
+      </c>
+      <c r="D589" t="n">
+        <v>1021.5</v>
+      </c>
+      <c r="E589" t="n">
+        <v>997</v>
+      </c>
+      <c r="F589" t="n">
+        <v>1213093212.5</v>
+      </c>
+      <c r="G589" t="n">
+        <v>1198615</v>
+      </c>
+      <c r="H589" t="n">
+        <v>3094</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="B590" t="n">
+        <v>1012</v>
+      </c>
+      <c r="C590" t="n">
+        <v>1009</v>
+      </c>
+      <c r="D590" t="n">
+        <v>1020</v>
+      </c>
+      <c r="E590" t="n">
+        <v>992</v>
+      </c>
+      <c r="F590" t="n">
+        <v>1184970660.5</v>
+      </c>
+      <c r="G590" t="n">
+        <v>1174635</v>
+      </c>
+      <c r="H590" t="n">
+        <v>2916</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="B591" t="n">
+        <v>1017</v>
+      </c>
+      <c r="C591" t="n">
+        <v>1005.5</v>
+      </c>
+      <c r="D591" t="n">
+        <v>1030.5</v>
+      </c>
+      <c r="E591" t="n">
+        <v>1002</v>
+      </c>
+      <c r="F591" t="n">
+        <v>236324736.5</v>
+      </c>
+      <c r="G591" t="n">
+        <v>5</v>
+      </c>
+      <c r="H591" t="n">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="B592" t="n">
+        <v>975</v>
+      </c>
+      <c r="C592" t="n">
+        <v>1014.5</v>
+      </c>
+      <c r="D592" t="n">
+        <v>1020</v>
+      </c>
+      <c r="E592" t="n">
+        <v>970</v>
+      </c>
+      <c r="F592" t="n">
+        <v>748776944.5</v>
+      </c>
+      <c r="G592" t="n">
+        <v>756508</v>
+      </c>
+      <c r="H592" t="n">
+        <v>3325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>